<commit_message>
"All tested, compiling to a .jar"
</commit_message>
<xml_diff>
--- a/src/main/resources/mainapp/reportTemplate.xlsx
+++ b/src/main/resources/mainapp/reportTemplate.xlsx
@@ -147,8 +147,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -449,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A3" sqref="A3:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -466,8 +468,8 @@
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -495,22 +497,247 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -520,10 +747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A3" sqref="A3:G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -537,7 +764,7 @@
     <col min="7" max="7" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="33" customHeight="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -572,22 +799,643 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -600,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -618,7 +1466,7 @@
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="33" customHeight="1">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -657,24 +1505,384 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -687,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E13"/>
+      <selection activeCell="A3" sqref="A3:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -704,7 +1912,7 @@
     <col min="7" max="7" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="17.399999999999999" customHeight="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -739,22 +1947,436 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -767,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -785,7 +2407,7 @@
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="21" customHeight="1">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="21" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
@@ -824,24 +2446,334 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fixes for H2 database
</commit_message>
<xml_diff>
--- a/src/main/resources/mainapp/reportTemplate.xlsx
+++ b/src/main/resources/mainapp/reportTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="13704" windowHeight="5424" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Истец_заявитель" sheetId="4" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Иные дела на контроле" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:G14"/>
 </workbook>
 </file>
 
@@ -46,18 +47,8 @@
 текущая ситуация</t>
   </si>
   <si>
-    <t>1. Дела, по которым министерство является истцом (заявителем)</t>
-  </si>
-  <si>
-    <t>2. Дела, по которым министерство является ответчиком (лицом, решения, действия либо бездействие которого оспариваются, заинтересованным лицом по делам особого производства)</t>
-  </si>
-  <si>
     <t>Ответчик 
 (заинт. лицо)</t>
-  </si>
-  <si>
-    <t>3. Дела, по которым министерство является третьим лицом (заинтересованным лицом по делам, 
-возникающим из административных правоотношений)</t>
   </si>
   <si>
     <t>4. Уголовные дела и дела об административных правонарушениях</t>
@@ -66,7 +57,17 @@
     <t>Лицо, в отношении которого ведется производство</t>
   </si>
   <si>
-    <t>5. Иные дела на контроле министерства</t>
+    <t>1. Дела, по которым наша компания является истцом (заявителем)</t>
+  </si>
+  <si>
+    <t>2. Дела, по которым наша компания является ответчиком (лицом, решения, действия либо бездействие которого оспариваются, заинтересованным лицом по делам особого производства)</t>
+  </si>
+  <si>
+    <t>3. Дела, по которым наша компания является третьим лицом (заинтересованным лицом по делам, 
+возникающим из административных правоотношений)</t>
+  </si>
+  <si>
+    <t>5. Иные дела на контроле</t>
   </si>
 </sst>
 </file>
@@ -453,9 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G29"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -470,7 +469,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="43.2" customHeight="1">
@@ -478,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -750,7 +749,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G73"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -766,7 +765,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1450,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1468,7 +1467,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1486,7 +1485,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -1914,7 +1913,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1928,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -2392,7 +2391,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2427,7 +2426,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>

</xml_diff>